<commit_message>
Add the task list for the week 31
</commit_message>
<xml_diff>
--- a/TASK_List.xlsx
+++ b/TASK_List.xlsx
@@ -5,16 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_documents\Task_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C78C1B-9EB5-4788-8DFE-6C11BFAA4955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7CCAF1-C203-4807-91B1-CC2776737A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week_24" sheetId="2" r:id="rId1"/>
     <sheet name="week_25" sheetId="1" r:id="rId2"/>
+    <sheet name="week_26" sheetId="3" r:id="rId3"/>
+    <sheet name="week_27" sheetId="4" r:id="rId4"/>
+    <sheet name="week_28" sheetId="5" r:id="rId5"/>
+    <sheet name="week_29" sheetId="6" r:id="rId6"/>
+    <sheet name="week_30" sheetId="7" r:id="rId7"/>
+    <sheet name="week_31" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
   <si>
     <t>Main task</t>
   </si>
@@ -75,9 +81,6 @@
     <t>Week 25</t>
   </si>
   <si>
-    <t>Testing LORA module</t>
-  </si>
-  <si>
     <t>Testing telimetry module</t>
   </si>
   <si>
@@ -121,6 +124,99 @@
   </si>
   <si>
     <t>On Hold</t>
+  </si>
+  <si>
+    <t>Task list week - 26</t>
+  </si>
+  <si>
+    <t>Drone mesurement</t>
+  </si>
+  <si>
+    <t>LORA Data rate test</t>
+  </si>
+  <si>
+    <t>Telimetry data rate test &amp; range test</t>
+  </si>
+  <si>
+    <t>Testing LORA module distance</t>
+  </si>
+  <si>
+    <t>Week 26</t>
+  </si>
+  <si>
+    <t>X-band</t>
+  </si>
+  <si>
+    <t>Review the layout of X-band</t>
+  </si>
+  <si>
+    <t>Delay due to weather condition</t>
+  </si>
+  <si>
+    <t>Task list week - 27</t>
+  </si>
+  <si>
+    <t>Testing the full system</t>
+  </si>
+  <si>
+    <t>Review the PCB layout of X-band</t>
+  </si>
+  <si>
+    <t>code merge</t>
+  </si>
+  <si>
+    <t>waiting for hardware</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing code on the hardware </t>
+  </si>
+  <si>
+    <t>Creat checklist for the PCB review</t>
+  </si>
+  <si>
+    <t>Final testing of V1 &amp; V2 board</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>waiting for the hardware</t>
+  </si>
+  <si>
+    <t>Add the software update to control the LDO of the power supply board</t>
+  </si>
+  <si>
+    <t>EEPROM function</t>
+  </si>
+  <si>
+    <t>Task list week - 30</t>
+  </si>
+  <si>
+    <t>Drone measurement</t>
+  </si>
+  <si>
+    <t>Corsair</t>
+  </si>
+  <si>
+    <t>Go through the data sheet of the SBC &amp; peripherals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hold due to issue in SDR power supply section </t>
+  </si>
+  <si>
+    <t>HOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cerbair </t>
+  </si>
+  <si>
+    <t>Task list week - 31</t>
   </si>
 </sst>
 </file>
@@ -152,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +285,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -515,11 +623,273 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,22 +1014,341 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -680,123 +1369,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1076,12 +1728,32 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{E367CB0A-873C-48CD-8C31-38AD088CE174}">
+  <we:reference id="wa200005107" version="1.1.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200005107" version="1.1.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5030E4-D589-4B9F-9E12-4F2B819987E2}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,196 +1769,146 @@
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-    </row>
-    <row r="2" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="60"/>
-      <c r="B2" s="48" t="s">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="155" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="157"/>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="167" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="54" t="s">
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="163"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="166"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="7">
+        <v>45091</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45092</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45093</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45094</v>
+      </c>
+      <c r="J6" s="10">
+        <v>45095</v>
+      </c>
+      <c r="K6" s="154"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="162">
+        <v>1</v>
+      </c>
+      <c r="C7" s="153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="49">
         <v>2</v>
       </c>
-      <c r="C5" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="51" t="s">
+      <c r="F7" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="45" t="s">
+      <c r="G7" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="162"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="55">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="66">
-        <v>45091</v>
-      </c>
-      <c r="G6" s="65">
-        <v>45092</v>
-      </c>
-      <c r="H6" s="65">
-        <v>45093</v>
-      </c>
-      <c r="I6" s="65">
-        <v>45094</v>
-      </c>
-      <c r="J6" s="70">
-        <v>45095</v>
-      </c>
-      <c r="K6" s="46"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
-      <c r="B7" s="43">
-        <v>1</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="80">
-        <v>2</v>
-      </c>
-      <c r="F7" s="81" t="s">
+      <c r="F8" s="56"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82" t="s">
+      <c r="K8" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="84" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="86">
-        <v>3</v>
-      </c>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="89" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="90" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="73"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="74"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="162"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="163"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1308,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1940,7 @@
     <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="3" customWidth="1"/>
@@ -1342,19 +1964,19 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="50"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="157"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -1365,35 +1987,35 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="164" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="45" t="s">
+      <c r="H6" s="159"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="160"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="153" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="44"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="58"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="154"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="172"/>
       <c r="G7" s="7">
         <v>45096</v>
       </c>
@@ -1412,13 +2034,13 @@
       <c r="L7" s="10">
         <v>45101</v>
       </c>
-      <c r="M7" s="46"/>
+      <c r="M7" s="154"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="43">
+      <c r="C8" s="162">
         <v>1</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="153" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -1432,7 +2054,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="26"/>
       <c r="M8" s="27" t="s">
@@ -1440,8 +2062,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
-      <c r="D9" s="47"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="161"/>
       <c r="E9" s="21" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +2076,7 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" s="34" t="s">
         <v>7</v>
@@ -1463,10 +2085,10 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="47"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="161"/>
       <c r="E10" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="16">
         <v>1</v>
@@ -1478,14 +2100,14 @@
       <c r="K10" s="17"/>
       <c r="L10" s="19"/>
       <c r="M10" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="46"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="154"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -1499,39 +2121,39 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="43">
+      <c r="C12" s="162">
         <v>2</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="153" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="29">
         <v>2</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="30"/>
       <c r="L12" s="32"/>
       <c r="M12" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="47"/>
+      <c r="C13" s="162"/>
+      <c r="D13" s="161"/>
       <c r="E13" s="15" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F13" s="16">
         <v>1</v>
@@ -1539,24 +2161,24 @@
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="19"/>
       <c r="M13" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="47"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="161"/>
       <c r="E14" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="16">
         <v>1</v>
@@ -1564,22 +2186,22 @@
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="19"/>
       <c r="M14" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="154"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
@@ -1593,14 +2215,14 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="43">
+      <c r="C16" s="162">
         <v>3</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="153" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>20</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>21</v>
       </c>
       <c r="F16" s="29">
         <v>1</v>
@@ -1609,25 +2231,25 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" s="32"/>
       <c r="M16" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="154"/>
       <c r="E17" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="42">
+        <v>21</v>
+      </c>
+      <c r="F17" s="40">
         <v>2</v>
       </c>
       <c r="G17" s="37"/>
@@ -1635,10 +2257,10 @@
       <c r="I17" s="38"/>
       <c r="J17" s="38"/>
       <c r="K17" s="37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M17" s="40" t="s">
         <v>7</v>
@@ -1692,6 +2314,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="M6:M7"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="D8:D11"/>
@@ -1700,13 +2327,1365 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D32143-F08C-44B7-9ED2-96F05E53CFD6}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="155" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="157"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="169" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="171" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="158" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="7">
+        <v>45103</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45104</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45105</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45106</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45107</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45108</v>
+      </c>
+      <c r="L6" s="154"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="164">
+        <v>1</v>
+      </c>
+      <c r="C7" s="153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="29">
+        <v>2</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="162"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="163"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="65">
+        <v>3</v>
+      </c>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="162">
+        <v>2</v>
+      </c>
+      <c r="C10" s="175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="71">
+        <v>1</v>
+      </c>
+      <c r="F10" s="72"/>
+      <c r="G10" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="173" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="174"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="162"/>
+      <c r="C11" s="175"/>
+      <c r="D11" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="77">
+        <v>1</v>
+      </c>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="79"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="173"/>
+      <c r="N11" s="174"/>
+    </row>
+    <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60">
+        <v>3</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="87" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="88">
+        <v>2</v>
+      </c>
+      <c r="F12" s="86"/>
+      <c r="G12" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="88" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="83">
+        <v>4</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="90" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="63">
+        <v>2</v>
+      </c>
+      <c r="F13" s="92"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="91"/>
+      <c r="L13" s="90"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BB936E-1321-4E1D-AB61-6515AD6BD114}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="155" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="157"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="169" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="171" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="158" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="7">
+        <v>45110</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45111</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45112</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45113</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45114</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45115</v>
+      </c>
+      <c r="L6" s="154"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="164">
+        <v>1</v>
+      </c>
+      <c r="C7" s="153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="104"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="162"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="99"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="99"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="163"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="162">
+        <v>2</v>
+      </c>
+      <c r="C10" s="175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="111">
+        <v>1</v>
+      </c>
+      <c r="F10" s="112"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="112"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="173" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="174"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="162"/>
+      <c r="C11" s="175"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="116"/>
+      <c r="M11" s="173"/>
+      <c r="N11" s="174"/>
+    </row>
+    <row r="12" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="96">
+        <v>3</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="88">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="178"/>
+      <c r="N12" s="178"/>
+      <c r="O12" s="178"/>
+    </row>
+    <row r="13" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="121"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="81"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="176" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="177"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96">
+        <v>4</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="88">
+        <v>2</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="108" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="123"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="M10:N11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E33FD2-08B6-48EA-975F-2BC8E396141E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C22414C-1EDB-4FDA-A59B-4CE28FC62E6B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64718D59-00D0-44E4-9F66-E543B5AD6EB3}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="155" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="157"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="169" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="171" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="158" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="7">
+        <v>45131</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45132</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45133</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45134</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45135</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45136</v>
+      </c>
+      <c r="L6" s="154"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="164">
+        <v>1</v>
+      </c>
+      <c r="C7" s="153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="173" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="174"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="163"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="173"/>
+      <c r="N8" s="174"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="97"/>
+      <c r="C9" s="180" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="152" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="133"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+    </row>
+    <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="162">
+        <v>2</v>
+      </c>
+      <c r="C10" s="175"/>
+      <c r="D10" s="150" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="146">
+        <v>1</v>
+      </c>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="148"/>
+      <c r="J10" s="147"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="146"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="162"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+    </row>
+    <row r="12" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="171">
+        <v>3</v>
+      </c>
+      <c r="C12" s="153" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="87" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="88">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="179"/>
+      <c r="C13" s="161"/>
+      <c r="D13" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="88">
+        <v>2</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="172"/>
+      <c r="C14" s="154"/>
+      <c r="D14" s="143" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="125">
+        <v>2</v>
+      </c>
+      <c r="F14" s="126"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="144"/>
+      <c r="L14" s="145" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="96">
+        <v>4</v>
+      </c>
+      <c r="C15" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="125"/>
+      <c r="E15" s="125"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="127"/>
+      <c r="L15" s="128"/>
+    </row>
+    <row r="16" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="123"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49D5F62-D26C-4867-BA36-B99065C69135}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="155" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="157"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="169" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="167" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="158" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="7">
+        <v>45138</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45139</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45140</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45141</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45142</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45143</v>
+      </c>
+      <c r="L6" s="154"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="164">
+        <v>1</v>
+      </c>
+      <c r="C7" s="153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="173" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="174"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="163"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="173"/>
+      <c r="N8" s="174"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="97"/>
+      <c r="C9" s="180" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="152"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+    </row>
+    <row r="10" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="162">
+        <v>2</v>
+      </c>
+      <c r="C10" s="175"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="146">
+        <v>1</v>
+      </c>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="148"/>
+      <c r="J10" s="147"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="146"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="162"/>
+      <c r="C11" s="181"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+    </row>
+    <row r="12" spans="1:15" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="171">
+        <v>3</v>
+      </c>
+      <c r="C12" s="153" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="182" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="183">
+        <v>1</v>
+      </c>
+      <c r="F12" s="184"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="185"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="186"/>
+      <c r="L12" s="187" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="173" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="174"/>
+      <c r="O12" s="174"/>
+    </row>
+    <row r="13" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="172"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="182" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="183">
+        <v>2</v>
+      </c>
+      <c r="F13" s="184"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="185"/>
+      <c r="K13" s="186"/>
+      <c r="L13" s="187" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96">
+        <v>4</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="125"/>
+      <c r="E14" s="125"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="128"/>
+    </row>
+    <row r="15" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="123"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update the task list for the week31 end
</commit_message>
<xml_diff>
--- a/TASK_List.xlsx
+++ b/TASK_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_documents\Task_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7CCAF1-C203-4807-91B1-CC2776737A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4C4BC-CAC3-45DF-BE9A-F04FFA5F39A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="64">
   <si>
     <t>Main task</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Go through the data sheet of the SBC &amp; peripherals</t>
   </si>
   <si>
-    <t xml:space="preserve">Hold due to issue in SDR power supply section </t>
-  </si>
-  <si>
     <t>HOLD</t>
   </si>
   <si>
@@ -217,6 +214,27 @@
   </si>
   <si>
     <t>Task list week - 31</t>
+  </si>
+  <si>
+    <t>jammer gun</t>
+  </si>
+  <si>
+    <t>update the firmware for plotting the frequency vs amplitude graph</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Read TPS2482 over the I2C reading current &amp; voltage</t>
+  </si>
+  <si>
+    <t>Add software patch for TPS2482</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Increase the transmission speed of the lora device</t>
   </si>
 </sst>
 </file>
@@ -248,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +315,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="48">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -885,11 +909,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1345,6 +1428,24 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1432,23 +1533,89 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1771,18 +1938,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="157"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="163"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -1793,34 +1960,34 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="165" t="s">
+      <c r="D5" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="167" t="s">
+      <c r="E5" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="164" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="153" t="s">
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="163"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="166"/>
-      <c r="E6" s="168"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="174"/>
       <c r="F6" s="7">
         <v>45091</v>
       </c>
@@ -1836,13 +2003,13 @@
       <c r="J6" s="10">
         <v>45095</v>
       </c>
-      <c r="K6" s="154"/>
+      <c r="K6" s="160"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="162">
+      <c r="B7" s="168">
         <v>1</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="159" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="48" t="s">
@@ -1865,8 +2032,8 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="162"/>
-      <c r="C8" s="161"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="54" t="s">
         <v>6</v>
       </c>
@@ -1887,8 +2054,8 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="162"/>
-      <c r="C9" s="161"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="167"/>
       <c r="D9" s="43"/>
       <c r="E9" s="47"/>
       <c r="F9" s="46"/>
@@ -1899,8 +2066,8 @@
       <c r="K9" s="45"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="163"/>
-      <c r="C10" s="154"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="160"/>
       <c r="D10" s="9"/>
       <c r="E10" s="14"/>
       <c r="F10" s="13"/>
@@ -1964,19 +2131,19 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="157"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="162"/>
+      <c r="M3" s="163"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -1987,35 +2154,35 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="153" t="s">
+      <c r="D6" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="169" t="s">
+      <c r="E6" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="171" t="s">
+      <c r="F6" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="158" t="s">
+      <c r="G6" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="160"/>
-      <c r="L6" s="160"/>
-      <c r="M6" s="153" t="s">
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="166"/>
+      <c r="L6" s="166"/>
+      <c r="M6" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="163"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="172"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="178"/>
       <c r="G7" s="7">
         <v>45096</v>
       </c>
@@ -2034,13 +2201,13 @@
       <c r="L7" s="10">
         <v>45101</v>
       </c>
-      <c r="M7" s="154"/>
+      <c r="M7" s="160"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="162">
+      <c r="C8" s="168">
         <v>1</v>
       </c>
-      <c r="D8" s="153" t="s">
+      <c r="D8" s="159" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -2062,8 +2229,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="162"/>
-      <c r="D9" s="161"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="167"/>
       <c r="E9" s="21" t="s">
         <v>6</v>
       </c>
@@ -2085,8 +2252,8 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="161"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="167"/>
       <c r="E10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2106,8 +2273,8 @@
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="154"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="160"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -2121,10 +2288,10 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="162">
+      <c r="C12" s="168">
         <v>2</v>
       </c>
-      <c r="D12" s="153" t="s">
+      <c r="D12" s="159" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="28" t="s">
@@ -2150,8 +2317,8 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="162"/>
-      <c r="D13" s="161"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="167"/>
       <c r="E13" s="15" t="s">
         <v>31</v>
       </c>
@@ -2175,8 +2342,8 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="161"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="167"/>
       <c r="E14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2200,8 +2367,8 @@
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="163"/>
-      <c r="D15" s="154"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="160"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
@@ -2215,10 +2382,10 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="162">
+      <c r="C16" s="168">
         <v>3</v>
       </c>
-      <c r="D16" s="153" t="s">
+      <c r="D16" s="159" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="28" t="s">
@@ -2244,8 +2411,8 @@
     <row r="17" spans="1:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="154"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="160"/>
       <c r="E17" s="41" t="s">
         <v>21</v>
       </c>
@@ -2369,19 +2536,19 @@
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="157"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="163"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2411,36 +2578,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="D5" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="171" t="s">
+      <c r="E5" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="153" t="s">
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="163"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="172"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="178"/>
       <c r="F6" s="7">
         <v>45103</v>
       </c>
@@ -2459,14 +2626,14 @@
       <c r="K6" s="10">
         <v>45108</v>
       </c>
-      <c r="L6" s="154"/>
+      <c r="L6" s="160"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="164">
+      <c r="B7" s="170">
         <v>1</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="159" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -2486,8 +2653,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="162"/>
-      <c r="C8" s="161"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="15" t="s">
         <v>16</v>
       </c>
@@ -2505,8 +2672,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="163"/>
-      <c r="C9" s="154"/>
+      <c r="B9" s="169"/>
+      <c r="C9" s="160"/>
       <c r="D9" s="64" t="s">
         <v>6</v>
       </c>
@@ -2526,10 +2693,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="162">
+      <c r="B10" s="168">
         <v>2</v>
       </c>
-      <c r="C10" s="175" t="s">
+      <c r="C10" s="181" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="70" t="s">
@@ -2549,14 +2716,14 @@
       <c r="L10" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="173" t="s">
+      <c r="M10" s="179" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="174"/>
+      <c r="N10" s="180"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="162"/>
-      <c r="C11" s="175"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="181"/>
       <c r="D11" s="76" t="s">
         <v>29</v>
       </c>
@@ -2574,8 +2741,8 @@
       <c r="L11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="173"/>
-      <c r="N11" s="174"/>
+      <c r="M11" s="179"/>
+      <c r="N11" s="180"/>
     </row>
     <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="60">
@@ -2695,19 +2862,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="157"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="163"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2737,36 +2904,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="D5" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="171" t="s">
+      <c r="E5" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="153" t="s">
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="163"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="172"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="178"/>
       <c r="F6" s="7">
         <v>45110</v>
       </c>
@@ -2785,14 +2952,14 @@
       <c r="K6" s="10">
         <v>45115</v>
       </c>
-      <c r="L6" s="154"/>
+      <c r="L6" s="160"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="164">
+      <c r="B7" s="170">
         <v>1</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="159" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="109" t="s">
@@ -2817,8 +2984,8 @@
       <c r="M7" s="104"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="162"/>
-      <c r="C8" s="161"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="98" t="s">
         <v>43</v>
       </c>
@@ -2832,8 +2999,8 @@
       <c r="L8" s="99"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="163"/>
-      <c r="C9" s="154"/>
+      <c r="B9" s="169"/>
+      <c r="C9" s="160"/>
       <c r="D9" s="103"/>
       <c r="E9" s="40"/>
       <c r="F9" s="37"/>
@@ -2845,10 +3012,10 @@
       <c r="L9" s="40"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="162">
+      <c r="B10" s="168">
         <v>2</v>
       </c>
-      <c r="C10" s="175" t="s">
+      <c r="C10" s="181" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="110" t="s">
@@ -2864,14 +3031,14 @@
       <c r="J10" s="112"/>
       <c r="K10" s="114"/>
       <c r="L10" s="111"/>
-      <c r="M10" s="173" t="s">
+      <c r="M10" s="179" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="174"/>
+      <c r="N10" s="180"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="162"/>
-      <c r="C11" s="175"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="181"/>
       <c r="D11" s="115"/>
       <c r="E11" s="116"/>
       <c r="F11" s="117"/>
@@ -2881,8 +3048,8 @@
       <c r="J11" s="117"/>
       <c r="K11" s="119"/>
       <c r="L11" s="116"/>
-      <c r="M11" s="173"/>
-      <c r="N11" s="174"/>
+      <c r="M11" s="179"/>
+      <c r="N11" s="180"/>
     </row>
     <row r="12" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="96">
@@ -2910,9 +3077,9 @@
       <c r="L12" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="178"/>
-      <c r="N12" s="178"/>
-      <c r="O12" s="178"/>
+      <c r="M12" s="184"/>
+      <c r="N12" s="184"/>
+      <c r="O12" s="184"/>
     </row>
     <row r="13" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="121"/>
@@ -2930,10 +3097,10 @@
       <c r="L13" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="176" t="s">
+      <c r="M13" s="182" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="177"/>
+      <c r="N13" s="183"/>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3034,7 +3201,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,19 +3231,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="161" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="157"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="163"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3106,36 +3273,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="D5" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="171" t="s">
+      <c r="E5" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="153" t="s">
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="163"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="172"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="178"/>
       <c r="F6" s="7">
         <v>45131</v>
       </c>
@@ -3154,14 +3321,14 @@
       <c r="K6" s="10">
         <v>45136</v>
       </c>
-      <c r="L6" s="154"/>
+      <c r="L6" s="160"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="164">
+      <c r="B7" s="170">
         <v>1</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="159" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="98" t="s">
@@ -3175,14 +3342,14 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="173" t="s">
+      <c r="M7" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="174"/>
+      <c r="N7" s="180"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="163"/>
-      <c r="C8" s="154"/>
+      <c r="B8" s="169"/>
+      <c r="C8" s="160"/>
       <c r="D8" s="138"/>
       <c r="E8" s="139"/>
       <c r="F8" s="140"/>
@@ -3192,12 +3359,12 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="173"/>
-      <c r="N8" s="174"/>
+      <c r="M8" s="179"/>
+      <c r="N8" s="180"/>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="180" t="s">
+      <c r="C9" s="186" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="152" t="s">
@@ -3215,10 +3382,10 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="162">
+      <c r="B10" s="168">
         <v>2</v>
       </c>
-      <c r="C10" s="175"/>
+      <c r="C10" s="181"/>
       <c r="D10" s="150" t="s">
         <v>37</v>
       </c>
@@ -3236,8 +3403,8 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="162"/>
-      <c r="C11" s="181"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="187"/>
       <c r="D11" s="151"/>
       <c r="E11" s="129"/>
       <c r="F11" s="130"/>
@@ -3251,10 +3418,10 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="171">
+      <c r="B12" s="177">
         <v>3</v>
       </c>
-      <c r="C12" s="153" t="s">
+      <c r="C12" s="159" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="87" t="s">
@@ -3278,8 +3445,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="179"/>
-      <c r="C13" s="161"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="167"/>
       <c r="D13" s="87" t="s">
         <v>49</v>
       </c>
@@ -3300,8 +3467,8 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="172"/>
-      <c r="C14" s="154"/>
+      <c r="B14" s="178"/>
+      <c r="C14" s="160"/>
       <c r="D14" s="143" t="s">
         <v>45</v>
       </c>
@@ -3375,10 +3542,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49D5F62-D26C-4867-BA36-B99065C69135}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3409,19 +3576,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="155" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="157"/>
+      <c r="B2" s="161" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="163"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3451,36 +3618,36 @@
     </row>
     <row r="5" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="D5" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="167" t="s">
+      <c r="E5" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="153" t="s">
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="163"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="168"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="200"/>
       <c r="F6" s="7">
         <v>45138</v>
       </c>
@@ -3499,20 +3666,20 @@
       <c r="K6" s="10">
         <v>45143</v>
       </c>
-      <c r="L6" s="154"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L6" s="160"/>
+    </row>
+    <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="164">
+      <c r="B7" s="170">
         <v>1</v>
       </c>
-      <c r="C7" s="153" t="s">
-        <v>4</v>
+      <c r="C7" s="188" t="s">
+        <v>57</v>
       </c>
       <c r="D7" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="99"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="100"/>
       <c r="G7" s="101"/>
       <c r="H7" s="101"/>
@@ -3520,16 +3687,16 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="173" t="s">
+      <c r="M7" s="211" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="174"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="163"/>
-      <c r="C8" s="154"/>
+      <c r="N7" s="180"/>
+    </row>
+    <row r="8" spans="1:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="169"/>
+      <c r="C8" s="189"/>
       <c r="D8" s="138"/>
-      <c r="E8" s="139"/>
+      <c r="E8" s="201"/>
       <c r="F8" s="140"/>
       <c r="G8" s="141"/>
       <c r="H8" s="141"/>
@@ -3537,146 +3704,208 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="173"/>
-      <c r="N8" s="174"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M8" s="211"/>
+      <c r="N8" s="180"/>
+    </row>
+    <row r="9" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="180" t="s">
+      <c r="C9" s="195" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="152"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="135"/>
-      <c r="H9" s="135"/>
-      <c r="I9" s="135"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="136"/>
-      <c r="L9" s="125"/>
+      <c r="D9" s="207" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="202">
+        <v>3</v>
+      </c>
+      <c r="F9" s="190"/>
+      <c r="G9" s="191" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="191"/>
+      <c r="I9" s="191"/>
+      <c r="J9" s="190" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="192"/>
+      <c r="L9" s="88" t="s">
+        <v>59</v>
+      </c>
       <c r="M9" s="124"/>
       <c r="N9" s="124"/>
     </row>
-    <row r="10" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="162">
+    <row r="10" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="168">
         <v>2</v>
       </c>
-      <c r="C10" s="175"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="146">
-        <v>1</v>
-      </c>
+      <c r="C10" s="196"/>
+      <c r="D10" s="209" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="203"/>
       <c r="F10" s="147"/>
       <c r="G10" s="148"/>
       <c r="H10" s="148"/>
       <c r="I10" s="148"/>
-      <c r="J10" s="147"/>
+      <c r="J10" s="147" t="s">
+        <v>24</v>
+      </c>
       <c r="K10" s="149"/>
-      <c r="L10" s="146"/>
+      <c r="L10" s="146" t="s">
+        <v>62</v>
+      </c>
       <c r="M10" s="137"/>
       <c r="N10" s="137"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="162"/>
-      <c r="C11" s="181"/>
-      <c r="D11" s="151"/>
-      <c r="E11" s="129"/>
+    <row r="11" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="168"/>
+      <c r="C11" s="197"/>
+      <c r="D11" s="208"/>
+      <c r="E11" s="204"/>
       <c r="F11" s="130"/>
       <c r="G11" s="131"/>
       <c r="H11" s="131"/>
       <c r="I11" s="131"/>
       <c r="J11" s="130"/>
       <c r="K11" s="132"/>
-      <c r="L11" s="139"/>
+      <c r="L11" s="129"/>
       <c r="M11" s="137"/>
       <c r="N11" s="137"/>
     </row>
-    <row r="12" spans="1:15" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="171">
+    <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="177">
         <v>3</v>
       </c>
-      <c r="C12" s="153" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="182" t="s">
+      <c r="C12" s="188" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="213" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="183">
+      <c r="E12" s="214">
         <v>1</v>
       </c>
-      <c r="F12" s="184"/>
-      <c r="G12" s="185"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="185"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="186"/>
-      <c r="L12" s="187" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="173" t="s">
+      <c r="F12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="180"/>
+      <c r="N12" s="180"/>
+      <c r="O12" s="180"/>
+    </row>
+    <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="185"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="215" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17">
+        <v>2</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
+      <c r="O13" s="124"/>
+    </row>
+    <row r="14" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="185"/>
+      <c r="C14" s="193"/>
+      <c r="D14" s="212" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="205"/>
+      <c r="F14" s="194"/>
+      <c r="G14" s="194"/>
+      <c r="H14" s="194"/>
+      <c r="I14" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="194"/>
+      <c r="K14" s="210"/>
+      <c r="L14" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+    </row>
+    <row r="15" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="178"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="154" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="206">
+        <v>2</v>
+      </c>
+      <c r="F15" s="156"/>
+      <c r="G15" s="157"/>
+      <c r="H15" s="157"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="157"/>
+      <c r="K15" s="158"/>
+      <c r="L15" s="155" t="s">
         <v>54</v>
       </c>
-      <c r="N12" s="174"/>
-      <c r="O12" s="174"/>
-    </row>
-    <row r="13" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="172"/>
-      <c r="C13" s="154"/>
-      <c r="D13" s="182" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="183">
-        <v>2</v>
-      </c>
-      <c r="F13" s="184"/>
-      <c r="G13" s="185"/>
-      <c r="H13" s="185"/>
-      <c r="I13" s="185"/>
-      <c r="J13" s="185"/>
-      <c r="K13" s="186"/>
-      <c r="L13" s="187" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="96">
+      <c r="M15" s="216"/>
+      <c r="N15" s="217"/>
+      <c r="O15" s="217"/>
+    </row>
+    <row r="16" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="96">
         <v>4</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C16" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="127"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="127"/>
-      <c r="K14" s="127"/>
-      <c r="L14" s="128"/>
-    </row>
-    <row r="15" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="123"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="125"/>
+    </row>
+    <row r="17" spans="2:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="198"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
@@ -3685,6 +3914,11 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Task list for the week32 is added
</commit_message>
<xml_diff>
--- a/TASK_List.xlsx
+++ b/TASK_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_documents\Task_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4C4BC-CAC3-45DF-BE9A-F04FFA5F39A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A6CDB5-9967-43E7-83B0-7E96D937637D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week_24" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="week_29" sheetId="6" r:id="rId6"/>
     <sheet name="week_30" sheetId="7" r:id="rId7"/>
     <sheet name="week_31" sheetId="8" r:id="rId8"/>
+    <sheet name="Week_32" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
   <si>
     <t>Main task</t>
   </si>
@@ -235,6 +236,12 @@
   </si>
   <si>
     <t>Increase the transmission speed of the lora device</t>
+  </si>
+  <si>
+    <t>Task list week - 32</t>
+  </si>
+  <si>
+    <t>Power supply board (TPS2482) debug</t>
   </si>
 </sst>
 </file>
@@ -972,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1446,6 +1453,60 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1536,22 +1597,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1561,62 +1618,34 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1938,18 +1967,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="163"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="183"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -1960,34 +1989,34 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="171" t="s">
+      <c r="D5" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="173" t="s">
+      <c r="E5" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="184" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="159" t="s">
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="169"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="174"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="194"/>
       <c r="F6" s="7">
         <v>45091</v>
       </c>
@@ -2003,13 +2032,13 @@
       <c r="J6" s="10">
         <v>45095</v>
       </c>
-      <c r="K6" s="160"/>
+      <c r="K6" s="180"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="168">
+      <c r="B7" s="188">
         <v>1</v>
       </c>
-      <c r="C7" s="159" t="s">
+      <c r="C7" s="179" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="48" t="s">
@@ -2032,8 +2061,8 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="168"/>
-      <c r="C8" s="167"/>
+      <c r="B8" s="188"/>
+      <c r="C8" s="187"/>
       <c r="D8" s="54" t="s">
         <v>6</v>
       </c>
@@ -2054,8 +2083,8 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="168"/>
-      <c r="C9" s="167"/>
+      <c r="B9" s="188"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="43"/>
       <c r="E9" s="47"/>
       <c r="F9" s="46"/>
@@ -2066,8 +2095,8 @@
       <c r="K9" s="45"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="169"/>
-      <c r="C10" s="160"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="180"/>
       <c r="D10" s="9"/>
       <c r="E10" s="14"/>
       <c r="F10" s="13"/>
@@ -2131,19 +2160,19 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="163"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
+      <c r="M3" s="183"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -2154,35 +2183,35 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="170" t="s">
+      <c r="C6" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="159" t="s">
+      <c r="D6" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="175" t="s">
+      <c r="E6" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="177" t="s">
+      <c r="F6" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="184" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="165"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="165"/>
-      <c r="K6" s="166"/>
-      <c r="L6" s="166"/>
-      <c r="M6" s="159" t="s">
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
+      <c r="M6" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="169"/>
-      <c r="D7" s="160"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="178"/>
+      <c r="C7" s="189"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="196"/>
+      <c r="F7" s="198"/>
       <c r="G7" s="7">
         <v>45096</v>
       </c>
@@ -2201,13 +2230,13 @@
       <c r="L7" s="10">
         <v>45101</v>
       </c>
-      <c r="M7" s="160"/>
+      <c r="M7" s="180"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="168">
+      <c r="C8" s="188">
         <v>1</v>
       </c>
-      <c r="D8" s="159" t="s">
+      <c r="D8" s="179" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -2229,8 +2258,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="168"/>
-      <c r="D9" s="167"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="187"/>
       <c r="E9" s="21" t="s">
         <v>6</v>
       </c>
@@ -2252,8 +2281,8 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="167"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="187"/>
       <c r="E10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2273,8 +2302,8 @@
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="160"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="180"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -2288,10 +2317,10 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="168">
+      <c r="C12" s="188">
         <v>2</v>
       </c>
-      <c r="D12" s="159" t="s">
+      <c r="D12" s="179" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="28" t="s">
@@ -2317,8 +2346,8 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="168"/>
-      <c r="D13" s="167"/>
+      <c r="C13" s="188"/>
+      <c r="D13" s="187"/>
       <c r="E13" s="15" t="s">
         <v>31</v>
       </c>
@@ -2342,8 +2371,8 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="168"/>
-      <c r="D14" s="167"/>
+      <c r="C14" s="188"/>
+      <c r="D14" s="187"/>
       <c r="E14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2367,8 +2396,8 @@
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="160"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="180"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
@@ -2382,10 +2411,10 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="168">
+      <c r="C16" s="188">
         <v>3</v>
       </c>
-      <c r="D16" s="159" t="s">
+      <c r="D16" s="179" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="28" t="s">
@@ -2411,8 +2440,8 @@
     <row r="17" spans="1:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="160"/>
+      <c r="C17" s="189"/>
+      <c r="D17" s="180"/>
       <c r="E17" s="41" t="s">
         <v>21</v>
       </c>
@@ -2481,11 +2510,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="M6:M7"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="D8:D11"/>
@@ -2494,6 +2518,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2536,19 +2565,19 @@
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="183"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2578,36 +2607,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="177" t="s">
+      <c r="E5" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="159" t="s">
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="178"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7">
         <v>45103</v>
       </c>
@@ -2626,14 +2655,14 @@
       <c r="K6" s="10">
         <v>45108</v>
       </c>
-      <c r="L6" s="160"/>
+      <c r="L6" s="180"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="170">
+      <c r="B7" s="190">
         <v>1</v>
       </c>
-      <c r="C7" s="159" t="s">
+      <c r="C7" s="179" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -2653,8 +2682,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="168"/>
-      <c r="C8" s="167"/>
+      <c r="B8" s="188"/>
+      <c r="C8" s="187"/>
       <c r="D8" s="15" t="s">
         <v>16</v>
       </c>
@@ -2672,8 +2701,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="169"/>
-      <c r="C9" s="160"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="180"/>
       <c r="D9" s="64" t="s">
         <v>6</v>
       </c>
@@ -2693,10 +2722,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="168">
+      <c r="B10" s="188">
         <v>2</v>
       </c>
-      <c r="C10" s="181" t="s">
+      <c r="C10" s="201" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="70" t="s">
@@ -2716,14 +2745,14 @@
       <c r="L10" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="179" t="s">
+      <c r="M10" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="180"/>
+      <c r="N10" s="200"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="C11" s="181"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="76" t="s">
         <v>29</v>
       </c>
@@ -2741,8 +2770,8 @@
       <c r="L11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="179"/>
-      <c r="N11" s="180"/>
+      <c r="M11" s="199"/>
+      <c r="N11" s="200"/>
     </row>
     <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="60">
@@ -2807,11 +2836,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2819,6 +2843,11 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2862,19 +2891,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="183"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2904,36 +2933,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="177" t="s">
+      <c r="E5" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="159" t="s">
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="178"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7">
         <v>45110</v>
       </c>
@@ -2952,14 +2981,14 @@
       <c r="K6" s="10">
         <v>45115</v>
       </c>
-      <c r="L6" s="160"/>
+      <c r="L6" s="180"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="170">
+      <c r="B7" s="190">
         <v>1</v>
       </c>
-      <c r="C7" s="159" t="s">
+      <c r="C7" s="179" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="109" t="s">
@@ -2984,8 +3013,8 @@
       <c r="M7" s="104"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="168"/>
-      <c r="C8" s="167"/>
+      <c r="B8" s="188"/>
+      <c r="C8" s="187"/>
       <c r="D8" s="98" t="s">
         <v>43</v>
       </c>
@@ -2999,8 +3028,8 @@
       <c r="L8" s="99"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="169"/>
-      <c r="C9" s="160"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="180"/>
       <c r="D9" s="103"/>
       <c r="E9" s="40"/>
       <c r="F9" s="37"/>
@@ -3012,10 +3041,10 @@
       <c r="L9" s="40"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="168">
+      <c r="B10" s="188">
         <v>2</v>
       </c>
-      <c r="C10" s="181" t="s">
+      <c r="C10" s="201" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="110" t="s">
@@ -3031,14 +3060,14 @@
       <c r="J10" s="112"/>
       <c r="K10" s="114"/>
       <c r="L10" s="111"/>
-      <c r="M10" s="179" t="s">
+      <c r="M10" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="180"/>
+      <c r="N10" s="200"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="C11" s="181"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="115"/>
       <c r="E11" s="116"/>
       <c r="F11" s="117"/>
@@ -3048,8 +3077,8 @@
       <c r="J11" s="117"/>
       <c r="K11" s="119"/>
       <c r="L11" s="116"/>
-      <c r="M11" s="179"/>
-      <c r="N11" s="180"/>
+      <c r="M11" s="199"/>
+      <c r="N11" s="200"/>
     </row>
     <row r="12" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="96">
@@ -3077,9 +3106,9 @@
       <c r="L12" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
-      <c r="O12" s="184"/>
+      <c r="M12" s="204"/>
+      <c r="N12" s="204"/>
+      <c r="O12" s="204"/>
     </row>
     <row r="13" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="121"/>
@@ -3097,10 +3126,10 @@
       <c r="L13" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="182" t="s">
+      <c r="M13" s="202" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="183"/>
+      <c r="N13" s="203"/>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3231,19 +3260,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="181" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="183"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3273,36 +3302,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="177" t="s">
+      <c r="E5" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="159" t="s">
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="160"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="178"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="7">
         <v>45131</v>
       </c>
@@ -3321,14 +3350,14 @@
       <c r="K6" s="10">
         <v>45136</v>
       </c>
-      <c r="L6" s="160"/>
+      <c r="L6" s="180"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="170">
+      <c r="B7" s="190">
         <v>1</v>
       </c>
-      <c r="C7" s="159" t="s">
+      <c r="C7" s="179" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="98" t="s">
@@ -3342,14 +3371,14 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="179" t="s">
+      <c r="M7" s="199" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="180"/>
+      <c r="N7" s="200"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="169"/>
-      <c r="C8" s="160"/>
+      <c r="B8" s="189"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="138"/>
       <c r="E8" s="139"/>
       <c r="F8" s="140"/>
@@ -3359,12 +3388,12 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="179"/>
-      <c r="N8" s="180"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="200"/>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="186" t="s">
+      <c r="C9" s="206" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="152" t="s">
@@ -3382,10 +3411,10 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="168">
+      <c r="B10" s="188">
         <v>2</v>
       </c>
-      <c r="C10" s="181"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="150" t="s">
         <v>37</v>
       </c>
@@ -3403,8 +3432,8 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="C11" s="187"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="207"/>
       <c r="D11" s="151"/>
       <c r="E11" s="129"/>
       <c r="F11" s="130"/>
@@ -3418,10 +3447,10 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="177">
+      <c r="B12" s="197">
         <v>3</v>
       </c>
-      <c r="C12" s="159" t="s">
+      <c r="C12" s="179" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="87" t="s">
@@ -3445,8 +3474,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="185"/>
-      <c r="C13" s="167"/>
+      <c r="B13" s="205"/>
+      <c r="C13" s="187"/>
       <c r="D13" s="87" t="s">
         <v>49</v>
       </c>
@@ -3467,8 +3496,8 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="178"/>
-      <c r="C14" s="160"/>
+      <c r="B14" s="198"/>
+      <c r="C14" s="180"/>
       <c r="D14" s="143" t="s">
         <v>45</v>
       </c>
@@ -3521,6 +3550,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -3528,13 +3564,6 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3544,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49D5F62-D26C-4867-BA36-B99065C69135}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M19" sqref="A1:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,19 +3605,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="181" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="183"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3618,36 +3647,36 @@
     </row>
     <row r="5" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="208" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="159" t="s">
+      <c r="D5" s="179" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="199" t="s">
+      <c r="E5" s="211" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="164" t="s">
+      <c r="F5" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="159" t="s">
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="179" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="189"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="200"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="210"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="212"/>
       <c r="F6" s="7">
         <v>45138</v>
       </c>
@@ -3666,14 +3695,14 @@
       <c r="K6" s="10">
         <v>45143</v>
       </c>
-      <c r="L6" s="160"/>
+      <c r="L6" s="180"/>
     </row>
     <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="170">
+      <c r="B7" s="190">
         <v>1</v>
       </c>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="208" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="98" t="s">
@@ -3687,16 +3716,16 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="211" t="s">
+      <c r="M7" s="200" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="180"/>
+      <c r="N7" s="200"/>
     </row>
     <row r="8" spans="1:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="169"/>
-      <c r="C8" s="189"/>
+      <c r="B8" s="189"/>
+      <c r="C8" s="210"/>
       <c r="D8" s="138"/>
-      <c r="E8" s="201"/>
+      <c r="E8" s="164"/>
       <c r="F8" s="140"/>
       <c r="G8" s="141"/>
       <c r="H8" s="141"/>
@@ -3704,30 +3733,30 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="211"/>
-      <c r="N8" s="180"/>
+      <c r="M8" s="200"/>
+      <c r="N8" s="200"/>
     </row>
     <row r="9" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="195" t="s">
+      <c r="C9" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="207" t="s">
+      <c r="D9" s="170" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="202">
+      <c r="E9" s="165">
         <v>3</v>
       </c>
-      <c r="F9" s="190"/>
-      <c r="G9" s="191" t="s">
+      <c r="F9" s="159"/>
+      <c r="G9" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="191"/>
-      <c r="I9" s="191"/>
-      <c r="J9" s="190" t="s">
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="192"/>
+      <c r="K9" s="161"/>
       <c r="L9" s="88" t="s">
         <v>59</v>
       </c>
@@ -3735,14 +3764,14 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="168">
+      <c r="B10" s="188">
         <v>2</v>
       </c>
-      <c r="C10" s="196"/>
-      <c r="D10" s="209" t="s">
+      <c r="C10" s="214"/>
+      <c r="D10" s="172" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="203"/>
+      <c r="E10" s="166"/>
       <c r="F10" s="147"/>
       <c r="G10" s="148"/>
       <c r="H10" s="148"/>
@@ -3758,10 +3787,10 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="C11" s="197"/>
-      <c r="D11" s="208"/>
-      <c r="E11" s="204"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="215"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="167"/>
       <c r="F11" s="130"/>
       <c r="G11" s="131"/>
       <c r="H11" s="131"/>
@@ -3773,16 +3802,16 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="177">
+      <c r="B12" s="197">
         <v>3</v>
       </c>
-      <c r="C12" s="188" t="s">
+      <c r="C12" s="208" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="213" t="s">
+      <c r="D12" s="175" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="214">
+      <c r="E12" s="176">
         <v>1</v>
       </c>
       <c r="F12" s="30" t="s">
@@ -3798,14 +3827,14 @@
       <c r="L12" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="180"/>
-      <c r="N12" s="180"/>
-      <c r="O12" s="180"/>
+      <c r="M12" s="200"/>
+      <c r="N12" s="200"/>
+      <c r="O12" s="200"/>
     </row>
     <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="185"/>
-      <c r="C13" s="193"/>
-      <c r="D13" s="215" t="s">
+      <c r="B13" s="205"/>
+      <c r="C13" s="209"/>
+      <c r="D13" s="177" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="17">
@@ -3829,20 +3858,20 @@
       <c r="O13" s="124"/>
     </row>
     <row r="14" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="185"/>
-      <c r="C14" s="193"/>
-      <c r="D14" s="212" t="s">
+      <c r="B14" s="205"/>
+      <c r="C14" s="209"/>
+      <c r="D14" s="174" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="205"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="162"/>
       <c r="I14" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="194"/>
-      <c r="K14" s="210"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="45" t="s">
         <v>62</v>
       </c>
@@ -3851,12 +3880,12 @@
       <c r="O14" s="124"/>
     </row>
     <row r="15" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="178"/>
-      <c r="C15" s="189"/>
+      <c r="B15" s="198"/>
+      <c r="C15" s="210"/>
       <c r="D15" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="206">
+      <c r="E15" s="169">
         <v>2</v>
       </c>
       <c r="F15" s="156"/>
@@ -3868,9 +3897,9 @@
       <c r="L15" s="155" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="216"/>
-      <c r="N15" s="217"/>
-      <c r="O15" s="217"/>
+      <c r="M15" s="178"/>
+      <c r="N15" s="178"/>
+      <c r="O15" s="178"/>
     </row>
     <row r="16" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="96">
@@ -3891,7 +3920,7 @@
     </row>
     <row r="17" spans="2:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
-      <c r="C17" s="198"/>
+      <c r="C17" s="163"/>
       <c r="D17" s="12"/>
       <c r="E17" s="123"/>
       <c r="F17" s="13"/>
@@ -3922,4 +3951,391 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7E3BB-DC3B-449E-86C6-DE69392E897A}">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="181" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="183"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="190" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="208" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="179" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="193" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="184" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="210"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="7">
+        <v>45145</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45146</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45147</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45148</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45149</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45150</v>
+      </c>
+      <c r="L6" s="180"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="190">
+        <v>1</v>
+      </c>
+      <c r="C7" s="208" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="200" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="200"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="189"/>
+      <c r="C8" s="210"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="200"/>
+      <c r="N8" s="200"/>
+    </row>
+    <row r="9" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="97"/>
+      <c r="C9" s="213" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="170" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="226">
+        <v>3</v>
+      </c>
+      <c r="F9" s="159"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="159"/>
+      <c r="K9" s="161"/>
+      <c r="L9" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+    </row>
+    <row r="10" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="188">
+        <v>2</v>
+      </c>
+      <c r="C10" s="214"/>
+      <c r="D10" s="216" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="99"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+    </row>
+    <row r="11" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="188"/>
+      <c r="C11" s="215"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+    </row>
+    <row r="12" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="197">
+        <v>3</v>
+      </c>
+      <c r="C12" s="208" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="175" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="33">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="200"/>
+      <c r="N12" s="200"/>
+      <c r="O12" s="200"/>
+    </row>
+    <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="205"/>
+      <c r="C13" s="209"/>
+      <c r="D13" s="177" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="20">
+        <v>2</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
+      <c r="O13" s="124"/>
+    </row>
+    <row r="14" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="205"/>
+      <c r="C14" s="209"/>
+      <c r="D14" s="216" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="99"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+    </row>
+    <row r="15" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="205"/>
+      <c r="C15" s="209"/>
+      <c r="D15" s="217" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="227"/>
+      <c r="F15" s="218"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="219"/>
+      <c r="K15" s="220"/>
+      <c r="L15" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
+    </row>
+    <row r="16" spans="1:15" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="198"/>
+      <c r="C16" s="210"/>
+      <c r="D16" s="221" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="225">
+        <v>2</v>
+      </c>
+      <c r="F16" s="222"/>
+      <c r="G16" s="223"/>
+      <c r="H16" s="223"/>
+      <c r="I16" s="223"/>
+      <c r="J16" s="223"/>
+      <c r="K16" s="224"/>
+      <c r="L16" s="225" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="178"/>
+      <c r="N16" s="178"/>
+      <c r="O16" s="178"/>
+    </row>
+    <row r="17" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="96">
+        <v>4</v>
+      </c>
+      <c r="C17" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="144"/>
+      <c r="L17" s="125"/>
+    </row>
+    <row r="18" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the task list for the week-33
</commit_message>
<xml_diff>
--- a/TASK_List.xlsx
+++ b/TASK_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_documents\Task_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A6CDB5-9967-43E7-83B0-7E96D937637D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A08155-FB9F-42D4-9A0C-AC486E727B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week_24" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="week_30" sheetId="7" r:id="rId7"/>
     <sheet name="week_31" sheetId="8" r:id="rId8"/>
     <sheet name="Week_32" sheetId="9" r:id="rId9"/>
+    <sheet name="week_33" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="67">
   <si>
     <t>Main task</t>
   </si>
@@ -238,10 +239,13 @@
     <t>Increase the transmission speed of the lora device</t>
   </si>
   <si>
-    <t>Task list week - 32</t>
-  </si>
-  <si>
-    <t>Power supply board (TPS2482) debug</t>
+    <t xml:space="preserve">Testing the power supply module </t>
+  </si>
+  <si>
+    <t>Task list week - 33</t>
+  </si>
+  <si>
+    <t>Power supply board testing process</t>
   </si>
 </sst>
 </file>
@@ -979,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1507,117 +1511,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1627,25 +1520,135 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1967,18 +1970,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="188"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -1989,34 +1992,34 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="191" t="s">
+      <c r="D5" s="196" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="193" t="s">
+      <c r="E5" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="189" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="179" t="s">
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="189"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="194"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="199"/>
       <c r="F6" s="7">
         <v>45091</v>
       </c>
@@ -2032,13 +2035,13 @@
       <c r="J6" s="10">
         <v>45095</v>
       </c>
-      <c r="K6" s="180"/>
+      <c r="K6" s="185"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="188">
+      <c r="B7" s="193">
         <v>1</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="184" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="48" t="s">
@@ -2061,8 +2064,8 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="188"/>
-      <c r="C8" s="187"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="54" t="s">
         <v>6</v>
       </c>
@@ -2083,8 +2086,8 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="188"/>
-      <c r="C9" s="187"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="43"/>
       <c r="E9" s="47"/>
       <c r="F9" s="46"/>
@@ -2095,8 +2098,8 @@
       <c r="K9" s="45"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="189"/>
-      <c r="C10" s="180"/>
+      <c r="B10" s="194"/>
+      <c r="C10" s="185"/>
       <c r="D10" s="9"/>
       <c r="E10" s="14"/>
       <c r="F10" s="13"/>
@@ -2117,6 +2120,331 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D446C0C-0CAB-4B2C-8615-A0E145C217CB}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="186" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="195" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="213" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="184" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="198" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="189" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="184" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="7">
+        <v>45152</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45153</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45154</v>
+      </c>
+      <c r="I6" s="6">
+        <v>45155</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45156</v>
+      </c>
+      <c r="K6" s="10">
+        <v>45157</v>
+      </c>
+      <c r="L6" s="185"/>
+    </row>
+    <row r="7" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="195">
+        <v>1</v>
+      </c>
+      <c r="C7" s="213" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="221" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="146"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="205" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="205"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="194"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="205"/>
+      <c r="N8" s="205"/>
+    </row>
+    <row r="9" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="193">
+        <v>2</v>
+      </c>
+      <c r="C9" s="219" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="99"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="137"/>
+      <c r="N9" s="137"/>
+    </row>
+    <row r="10" spans="1:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="193"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="131"/>
+      <c r="I10" s="131"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+    </row>
+    <row r="11" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="210"/>
+      <c r="C11" s="214" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
+      <c r="O11" s="124"/>
+    </row>
+    <row r="12" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="210"/>
+      <c r="C12" s="214"/>
+      <c r="D12" s="180" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="99">
+        <v>2</v>
+      </c>
+      <c r="F12" s="181"/>
+      <c r="G12" s="182"/>
+      <c r="H12" s="101" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="101"/>
+      <c r="J12" s="182"/>
+      <c r="K12" s="183"/>
+      <c r="L12" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="124"/>
+      <c r="N12" s="124"/>
+      <c r="O12" s="124"/>
+    </row>
+    <row r="13" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="203"/>
+      <c r="C13" s="215"/>
+      <c r="D13" s="222" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="223">
+        <v>3</v>
+      </c>
+      <c r="F13" s="224"/>
+      <c r="G13" s="225"/>
+      <c r="H13" s="225"/>
+      <c r="I13" s="225"/>
+      <c r="J13" s="225"/>
+      <c r="K13" s="226"/>
+      <c r="L13" s="223" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="178"/>
+      <c r="N13" s="178"/>
+      <c r="O13" s="178"/>
+    </row>
+    <row r="14" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96">
+        <v>4</v>
+      </c>
+      <c r="C14" s="153" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="125"/>
+      <c r="E14" s="125"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="144"/>
+      <c r="L14" s="125"/>
+    </row>
+    <row r="15" spans="1:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2160,19 +2488,19 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="183"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="188"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -2183,35 +2511,35 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="190" t="s">
+      <c r="C6" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="179" t="s">
+      <c r="D6" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="195" t="s">
+      <c r="E6" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="197" t="s">
+      <c r="F6" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="184" t="s">
+      <c r="G6" s="189" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="185"/>
-      <c r="I6" s="185"/>
-      <c r="J6" s="185"/>
-      <c r="K6" s="186"/>
-      <c r="L6" s="186"/>
-      <c r="M6" s="179" t="s">
+      <c r="H6" s="190"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="190"/>
+      <c r="K6" s="191"/>
+      <c r="L6" s="191"/>
+      <c r="M6" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="189"/>
-      <c r="D7" s="180"/>
-      <c r="E7" s="196"/>
-      <c r="F7" s="198"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="201"/>
+      <c r="F7" s="203"/>
       <c r="G7" s="7">
         <v>45096</v>
       </c>
@@ -2230,13 +2558,13 @@
       <c r="L7" s="10">
         <v>45101</v>
       </c>
-      <c r="M7" s="180"/>
+      <c r="M7" s="185"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="188">
+      <c r="C8" s="193">
         <v>1</v>
       </c>
-      <c r="D8" s="179" t="s">
+      <c r="D8" s="184" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -2258,8 +2586,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="188"/>
-      <c r="D9" s="187"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="192"/>
       <c r="E9" s="21" t="s">
         <v>6</v>
       </c>
@@ -2281,8 +2609,8 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="188"/>
-      <c r="D10" s="187"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="192"/>
       <c r="E10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2302,8 +2630,8 @@
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="189"/>
-      <c r="D11" s="180"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="185"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
@@ -2317,10 +2645,10 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="188">
+      <c r="C12" s="193">
         <v>2</v>
       </c>
-      <c r="D12" s="179" t="s">
+      <c r="D12" s="184" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="28" t="s">
@@ -2346,8 +2674,8 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="188"/>
-      <c r="D13" s="187"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="192"/>
       <c r="E13" s="15" t="s">
         <v>31</v>
       </c>
@@ -2371,8 +2699,8 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="188"/>
-      <c r="D14" s="187"/>
+      <c r="C14" s="193"/>
+      <c r="D14" s="192"/>
       <c r="E14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2396,8 +2724,8 @@
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="189"/>
-      <c r="D15" s="180"/>
+      <c r="C15" s="194"/>
+      <c r="D15" s="185"/>
       <c r="E15" s="9"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
@@ -2411,10 +2739,10 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="188">
+      <c r="C16" s="193">
         <v>3</v>
       </c>
-      <c r="D16" s="179" t="s">
+      <c r="D16" s="184" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="28" t="s">
@@ -2440,8 +2768,8 @@
     <row r="17" spans="1:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
-      <c r="C17" s="189"/>
-      <c r="D17" s="180"/>
+      <c r="C17" s="194"/>
+      <c r="D17" s="185"/>
       <c r="E17" s="41" t="s">
         <v>21</v>
       </c>
@@ -2510,6 +2838,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="M6:M7"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="D8:D11"/>
@@ -2518,11 +2851,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2565,19 +2893,19 @@
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2607,36 +2935,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="195" t="s">
+      <c r="D5" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="179" t="s">
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="198"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="201"/>
+      <c r="E6" s="203"/>
       <c r="F6" s="7">
         <v>45103</v>
       </c>
@@ -2655,14 +2983,14 @@
       <c r="K6" s="10">
         <v>45108</v>
       </c>
-      <c r="L6" s="180"/>
+      <c r="L6" s="185"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="190">
+      <c r="B7" s="195">
         <v>1</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="184" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -2682,8 +3010,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="188"/>
-      <c r="C8" s="187"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="15" t="s">
         <v>16</v>
       </c>
@@ -2701,8 +3029,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="189"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="185"/>
       <c r="D9" s="64" t="s">
         <v>6</v>
       </c>
@@ -2722,10 +3050,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="188">
+      <c r="B10" s="193">
         <v>2</v>
       </c>
-      <c r="C10" s="201" t="s">
+      <c r="C10" s="206" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="70" t="s">
@@ -2745,14 +3073,14 @@
       <c r="L10" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="199" t="s">
+      <c r="M10" s="204" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="200"/>
+      <c r="N10" s="205"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188"/>
-      <c r="C11" s="201"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="76" t="s">
         <v>29</v>
       </c>
@@ -2770,8 +3098,8 @@
       <c r="L11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="199"/>
-      <c r="N11" s="200"/>
+      <c r="M11" s="204"/>
+      <c r="N11" s="205"/>
     </row>
     <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="60">
@@ -2836,6 +3164,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2843,11 +3176,6 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2891,19 +3219,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2933,36 +3261,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="195" t="s">
+      <c r="D5" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="179" t="s">
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="198"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="201"/>
+      <c r="E6" s="203"/>
       <c r="F6" s="7">
         <v>45110</v>
       </c>
@@ -2981,14 +3309,14 @@
       <c r="K6" s="10">
         <v>45115</v>
       </c>
-      <c r="L6" s="180"/>
+      <c r="L6" s="185"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="190">
+      <c r="B7" s="195">
         <v>1</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="184" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="109" t="s">
@@ -3013,8 +3341,8 @@
       <c r="M7" s="104"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="188"/>
-      <c r="C8" s="187"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="98" t="s">
         <v>43</v>
       </c>
@@ -3028,8 +3356,8 @@
       <c r="L8" s="99"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="189"/>
-      <c r="C9" s="180"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="185"/>
       <c r="D9" s="103"/>
       <c r="E9" s="40"/>
       <c r="F9" s="37"/>
@@ -3041,10 +3369,10 @@
       <c r="L9" s="40"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="188">
+      <c r="B10" s="193">
         <v>2</v>
       </c>
-      <c r="C10" s="201" t="s">
+      <c r="C10" s="206" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="110" t="s">
@@ -3060,14 +3388,14 @@
       <c r="J10" s="112"/>
       <c r="K10" s="114"/>
       <c r="L10" s="111"/>
-      <c r="M10" s="199" t="s">
+      <c r="M10" s="204" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="200"/>
+      <c r="N10" s="205"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188"/>
-      <c r="C11" s="201"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="115"/>
       <c r="E11" s="116"/>
       <c r="F11" s="117"/>
@@ -3077,8 +3405,8 @@
       <c r="J11" s="117"/>
       <c r="K11" s="119"/>
       <c r="L11" s="116"/>
-      <c r="M11" s="199"/>
-      <c r="N11" s="200"/>
+      <c r="M11" s="204"/>
+      <c r="N11" s="205"/>
     </row>
     <row r="12" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="96">
@@ -3106,9 +3434,9 @@
       <c r="L12" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="204"/>
-      <c r="N12" s="204"/>
-      <c r="O12" s="204"/>
+      <c r="M12" s="209"/>
+      <c r="N12" s="209"/>
+      <c r="O12" s="209"/>
     </row>
     <row r="13" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="121"/>
@@ -3126,10 +3454,10 @@
       <c r="L13" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="202" t="s">
+      <c r="M13" s="207" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="203"/>
+      <c r="N13" s="208"/>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3260,19 +3588,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3302,36 +3630,36 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="195" t="s">
+      <c r="D5" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="202" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="179" t="s">
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="198"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="201"/>
+      <c r="E6" s="203"/>
       <c r="F6" s="7">
         <v>45131</v>
       </c>
@@ -3350,14 +3678,14 @@
       <c r="K6" s="10">
         <v>45136</v>
       </c>
-      <c r="L6" s="180"/>
+      <c r="L6" s="185"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="190">
+      <c r="B7" s="195">
         <v>1</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="184" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="98" t="s">
@@ -3371,14 +3699,14 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="199" t="s">
+      <c r="M7" s="204" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="200"/>
+      <c r="N7" s="205"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="189"/>
-      <c r="C8" s="180"/>
+      <c r="B8" s="194"/>
+      <c r="C8" s="185"/>
       <c r="D8" s="138"/>
       <c r="E8" s="139"/>
       <c r="F8" s="140"/>
@@ -3388,12 +3716,12 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="199"/>
-      <c r="N8" s="200"/>
+      <c r="M8" s="204"/>
+      <c r="N8" s="205"/>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="206" t="s">
+      <c r="C9" s="211" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="152" t="s">
@@ -3411,10 +3739,10 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="188">
+      <c r="B10" s="193">
         <v>2</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="150" t="s">
         <v>37</v>
       </c>
@@ -3432,8 +3760,8 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188"/>
-      <c r="C11" s="207"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="212"/>
       <c r="D11" s="151"/>
       <c r="E11" s="129"/>
       <c r="F11" s="130"/>
@@ -3447,10 +3775,10 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="197">
+      <c r="B12" s="202">
         <v>3</v>
       </c>
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="184" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="87" t="s">
@@ -3474,8 +3802,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="205"/>
-      <c r="C13" s="187"/>
+      <c r="B13" s="210"/>
+      <c r="C13" s="192"/>
       <c r="D13" s="87" t="s">
         <v>49</v>
       </c>
@@ -3496,8 +3824,8 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="198"/>
-      <c r="C14" s="180"/>
+      <c r="B14" s="203"/>
+      <c r="C14" s="185"/>
       <c r="D14" s="143" t="s">
         <v>45</v>
       </c>
@@ -3550,6 +3878,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="M7:N8"/>
@@ -3557,13 +3892,6 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3573,8 +3901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49D5F62-D26C-4867-BA36-B99065C69135}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="A1:O19"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,19 +3933,19 @@
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -3647,36 +3975,36 @@
     </row>
     <row r="5" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="208" t="s">
+      <c r="C5" s="213" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="179" t="s">
+      <c r="D5" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="211" t="s">
+      <c r="E5" s="216" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="184" t="s">
+      <c r="F5" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="179" t="s">
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+      <c r="L5" s="184" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="210"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="212"/>
+      <c r="B6" s="194"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="217"/>
       <c r="F6" s="7">
         <v>45138</v>
       </c>
@@ -3695,14 +4023,14 @@
       <c r="K6" s="10">
         <v>45143</v>
       </c>
-      <c r="L6" s="180"/>
+      <c r="L6" s="185"/>
     </row>
     <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="190">
+      <c r="B7" s="195">
         <v>1</v>
       </c>
-      <c r="C7" s="208" t="s">
+      <c r="C7" s="213" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="98" t="s">
@@ -3716,14 +4044,14 @@
       <c r="J7" s="100"/>
       <c r="K7" s="102"/>
       <c r="L7" s="99"/>
-      <c r="M7" s="200" t="s">
+      <c r="M7" s="205" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="200"/>
+      <c r="N7" s="205"/>
     </row>
     <row r="8" spans="1:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="189"/>
-      <c r="C8" s="210"/>
+      <c r="B8" s="194"/>
+      <c r="C8" s="215"/>
       <c r="D8" s="138"/>
       <c r="E8" s="164"/>
       <c r="F8" s="140"/>
@@ -3733,12 +4061,12 @@
       <c r="J8" s="141"/>
       <c r="K8" s="142"/>
       <c r="L8" s="139"/>
-      <c r="M8" s="200"/>
-      <c r="N8" s="200"/>
+      <c r="M8" s="205"/>
+      <c r="N8" s="205"/>
     </row>
     <row r="9" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="97"/>
-      <c r="C9" s="213" t="s">
+      <c r="C9" s="218" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="170" t="s">
@@ -3764,10 +4092,10 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="188">
+      <c r="B10" s="193">
         <v>2</v>
       </c>
-      <c r="C10" s="214"/>
+      <c r="C10" s="219"/>
       <c r="D10" s="172" t="s">
         <v>63</v>
       </c>
@@ -3787,8 +4115,8 @@
       <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188"/>
-      <c r="C11" s="215"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="220"/>
       <c r="D11" s="171"/>
       <c r="E11" s="167"/>
       <c r="F11" s="130"/>
@@ -3802,10 +4130,10 @@
       <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="197">
+      <c r="B12" s="202">
         <v>3</v>
       </c>
-      <c r="C12" s="208" t="s">
+      <c r="C12" s="213" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="175" t="s">
@@ -3827,13 +4155,13 @@
       <c r="L12" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="200"/>
-      <c r="N12" s="200"/>
-      <c r="O12" s="200"/>
+      <c r="M12" s="205"/>
+      <c r="N12" s="205"/>
+      <c r="O12" s="205"/>
     </row>
     <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="205"/>
-      <c r="C13" s="209"/>
+      <c r="B13" s="210"/>
+      <c r="C13" s="214"/>
       <c r="D13" s="177" t="s">
         <v>60</v>
       </c>
@@ -3858,8 +4186,8 @@
       <c r="O13" s="124"/>
     </row>
     <row r="14" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="205"/>
-      <c r="C14" s="209"/>
+      <c r="B14" s="210"/>
+      <c r="C14" s="214"/>
       <c r="D14" s="174" t="s">
         <v>61</v>
       </c>
@@ -3880,8 +4208,8 @@
       <c r="O14" s="124"/>
     </row>
     <row r="15" spans="1:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="198"/>
-      <c r="C15" s="210"/>
+      <c r="B15" s="203"/>
+      <c r="C15" s="215"/>
       <c r="D15" s="154" t="s">
         <v>45</v>
       </c>
@@ -3955,10 +4283,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7E3BB-DC3B-449E-86C6-DE69392E897A}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A9:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,368 +4302,17 @@
     <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="181" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="190" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="208" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="179" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="193" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="184" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="179" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="210"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="7">
-        <v>45145</v>
-      </c>
-      <c r="G6" s="6">
-        <v>45146</v>
-      </c>
-      <c r="H6" s="6">
-        <v>45147</v>
-      </c>
-      <c r="I6" s="6">
-        <v>45148</v>
-      </c>
-      <c r="J6" s="7">
-        <v>45149</v>
-      </c>
-      <c r="K6" s="10">
-        <v>45150</v>
-      </c>
-      <c r="L6" s="180"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="190">
-        <v>1</v>
-      </c>
-      <c r="C7" s="208" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="200" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="200"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="189"/>
-      <c r="C8" s="210"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="141"/>
-      <c r="H8" s="141"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="142"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="200"/>
-      <c r="N8" s="200"/>
-    </row>
-    <row r="9" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="97"/>
-      <c r="C9" s="213" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="170" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="226">
-        <v>3</v>
-      </c>
-      <c r="F9" s="159"/>
-      <c r="G9" s="160"/>
-      <c r="H9" s="160"/>
-      <c r="I9" s="160"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="88" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-    </row>
-    <row r="10" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="188">
-        <v>2</v>
-      </c>
-      <c r="C10" s="214"/>
-      <c r="D10" s="216" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="102"/>
-      <c r="L10" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" s="137"/>
-      <c r="N10" s="137"/>
-    </row>
-    <row r="11" spans="1:15" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="188"/>
-      <c r="C11" s="215"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-    </row>
-    <row r="12" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="197">
-        <v>3</v>
-      </c>
-      <c r="C12" s="208" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="175" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="33">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" s="200"/>
-      <c r="N12" s="200"/>
-      <c r="O12" s="200"/>
-    </row>
-    <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="205"/>
-      <c r="C13" s="209"/>
-      <c r="D13" s="177" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="20">
-        <v>2</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-    </row>
-    <row r="14" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="205"/>
-      <c r="C14" s="209"/>
-      <c r="D14" s="216" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-    </row>
-    <row r="15" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="205"/>
-      <c r="C15" s="209"/>
-      <c r="D15" s="217" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="227"/>
-      <c r="F15" s="218"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="219"/>
-      <c r="K15" s="220"/>
-      <c r="L15" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-    </row>
-    <row r="16" spans="1:15" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="198"/>
-      <c r="C16" s="210"/>
-      <c r="D16" s="221" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="225">
-        <v>2</v>
-      </c>
-      <c r="F16" s="222"/>
-      <c r="G16" s="223"/>
-      <c r="H16" s="223"/>
-      <c r="I16" s="223"/>
-      <c r="J16" s="223"/>
-      <c r="K16" s="224"/>
-      <c r="L16" s="225" t="s">
-        <v>54</v>
-      </c>
-      <c r="M16" s="178"/>
-      <c r="N16" s="178"/>
-      <c r="O16" s="178"/>
-    </row>
-    <row r="17" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="96">
-        <v>4</v>
-      </c>
-      <c r="C17" s="153" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="125"/>
-    </row>
-    <row r="18" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="163"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12"/>
-    </row>
+    <row r="9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:L6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>